<commit_message>
Last adapptions befor test
</commit_message>
<xml_diff>
--- a/01_Calculations and Definitions/Message Definitions.xlsx
+++ b/01_Calculations and Definitions/Message Definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\JujuBot_uC_A8\01_Calculations and Definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9FE382-38AA-486C-A0EE-3AA7E5C90455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAB74C6-01E3-4429-9D92-2E73573EFD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="12220" windowHeight="17760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="28800" windowHeight="15910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -449,6 +449,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -761,60 +764,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
-      <c r="O1" s="30" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="33"/>
+      <c r="O1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="33"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="P2" s="29" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="P2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
     </row>
     <row r="3" spans="1:26" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
@@ -1913,7 +1916,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6:Z6"/>
+      <selection activeCell="N6" sqref="N6:Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1928,60 +1931,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
-      <c r="O1" s="30" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="33"/>
+      <c r="O1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="33"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="P2" s="29" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="P2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
     </row>
     <row r="3" spans="1:27" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
@@ -2244,13 +2247,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="15">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="D6" s="15">
         <v>0</v>
       </c>
       <c r="E6" s="15">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F6" s="15">
         <v>3</v>
@@ -2259,7 +2262,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="15">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="I6" s="15">
         <v>1</v>
@@ -2275,7 +2278,7 @@
       </c>
       <c r="M6" s="11">
         <f t="shared" ref="M6:M11" si="2">_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(C6,D6),E6),F6),G6),H6),I6),J6),K6),L6)</f>
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="O6" s="8" t="str">
         <f>DEC2HEX(B6,2)</f>
@@ -2283,7 +2286,7 @@
       </c>
       <c r="P6" s="14" t="str">
         <f>DEC2HEX(C6,2)</f>
-        <v>3C</v>
+        <v>6E</v>
       </c>
       <c r="Q6" s="14" t="str">
         <f t="shared" ref="Q6:Z8" si="3">DEC2HEX(D6,2)</f>
@@ -2291,7 +2294,7 @@
       </c>
       <c r="R6" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>01</v>
+        <v>14</v>
       </c>
       <c r="S6" s="14" t="str">
         <f t="shared" si="3"/>
@@ -2303,7 +2306,7 @@
       </c>
       <c r="U6" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="V6" s="14" t="str">
         <f t="shared" si="3"/>
@@ -2323,7 +2326,7 @@
       </c>
       <c r="Z6" s="11" t="str">
         <f>DEC2HEX(M6,2)</f>
-        <v>3C</v>
+        <v>4F</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
@@ -2331,45 +2334,45 @@
         <v>55</v>
       </c>
       <c r="B7" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="16">
         <v>185</v>
       </c>
-      <c r="D7" s="16">
-        <v>0</v>
-      </c>
-      <c r="E7" s="16">
-        <v>1</v>
-      </c>
-      <c r="F7" s="16">
-        <v>10</v>
-      </c>
-      <c r="G7" s="16">
-        <v>10</v>
-      </c>
-      <c r="H7" s="16">
+      <c r="D7" s="29">
+        <v>0</v>
+      </c>
+      <c r="E7" s="29">
+        <v>40</v>
+      </c>
+      <c r="F7" s="29">
+        <v>3</v>
+      </c>
+      <c r="G7" s="29">
+        <v>3</v>
+      </c>
+      <c r="H7" s="29">
+        <v>32</v>
+      </c>
+      <c r="I7" s="29">
+        <v>1</v>
+      </c>
+      <c r="J7" s="29">
         <v>20</v>
       </c>
-      <c r="I7" s="16">
-        <v>1</v>
-      </c>
-      <c r="J7" s="16">
-        <v>20</v>
-      </c>
-      <c r="K7" s="16">
-        <v>10</v>
-      </c>
-      <c r="L7" s="16">
-        <v>10</v>
+      <c r="K7" s="29">
+        <v>3</v>
+      </c>
+      <c r="L7" s="29">
+        <v>3</v>
       </c>
       <c r="M7" s="11">
         <f t="shared" si="2"/>
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="O7" s="8" t="str">
         <f t="shared" ref="O7:P8" si="4">DEC2HEX(B7,2)</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="P7" s="14" t="str">
         <f t="shared" si="4"/>
@@ -2381,19 +2384,19 @@
       </c>
       <c r="R7" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>01</v>
+        <v>28</v>
       </c>
       <c r="S7" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="T7" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="U7" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="V7" s="14" t="str">
         <f t="shared" si="3"/>
@@ -2405,15 +2408,15 @@
       </c>
       <c r="X7" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="Y7" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="Z7" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>B9</v>
+        <v>A4</v>
       </c>
     </row>
     <row r="8" spans="1:27" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2421,7 +2424,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="7">
         <v>54</v>
@@ -2430,16 +2433,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F8" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G8" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H8" s="7">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="I8" s="7">
         <v>1</v>
@@ -2448,18 +2451,18 @@
         <v>20</v>
       </c>
       <c r="K8" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L8" s="7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M8" s="12">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="O8" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="P8" s="7" t="str">
         <f t="shared" si="4"/>
@@ -2471,19 +2474,19 @@
       </c>
       <c r="R8" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>1E</v>
+        <v>14</v>
       </c>
       <c r="S8" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="T8" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="U8" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="V8" s="7" t="str">
         <f t="shared" si="3"/>
@@ -2495,15 +2498,15 @@
       </c>
       <c r="X8" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="Y8" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>0A</v>
+        <v>03</v>
       </c>
       <c r="Z8" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -2516,31 +2519,31 @@
       <c r="C9" s="15">
         <v>185</v>
       </c>
-      <c r="D9" s="15">
-        <v>0</v>
-      </c>
-      <c r="E9" s="15">
-        <v>10</v>
-      </c>
-      <c r="F9" s="15">
-        <v>10</v>
-      </c>
-      <c r="G9" s="15">
-        <v>10</v>
-      </c>
-      <c r="H9" s="15">
+      <c r="D9" s="29">
+        <v>0</v>
+      </c>
+      <c r="E9" s="29">
+        <v>10</v>
+      </c>
+      <c r="F9" s="29">
+        <v>10</v>
+      </c>
+      <c r="G9" s="29">
+        <v>10</v>
+      </c>
+      <c r="H9" s="29">
         <v>20</v>
       </c>
-      <c r="I9" s="15">
-        <v>1</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="I9" s="29">
+        <v>1</v>
+      </c>
+      <c r="J9" s="29">
         <v>20</v>
       </c>
-      <c r="K9" s="15">
-        <v>10</v>
-      </c>
-      <c r="L9" s="15">
+      <c r="K9" s="29">
+        <v>10</v>
+      </c>
+      <c r="L9" s="29">
         <v>10</v>
       </c>
       <c r="M9" s="11">
@@ -2601,7 +2604,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="15">
         <v>54</v>
@@ -2639,7 +2642,7 @@
       </c>
       <c r="O10" s="8" t="str">
         <f t="shared" ref="O10:O11" si="14">DEC2HEX(B10,2)</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="P10" s="15" t="str">
         <f t="shared" ref="P10:P11" si="15">DEC2HEX(C10,2)</f>
@@ -2691,7 +2694,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="7">
         <v>60</v>
@@ -2729,7 +2732,7 @@
       </c>
       <c r="O11" s="9" t="str">
         <f t="shared" si="14"/>
-        <v>03</v>
+        <v>01</v>
       </c>
       <c r="P11" s="7" t="str">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
defining interfaces of COM modules (in progress)
</commit_message>
<xml_diff>
--- a/01_Calculations and Definitions/Message Definitions.xlsx
+++ b/01_Calculations and Definitions/Message Definitions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\JujuBot_uC_A8\01_Calculations and Definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAB74C6-01E3-4429-9D92-2E73573EFD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9AE309-452D-433D-9847-4A2B78BD763C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="2620" windowWidth="28800" windowHeight="15910" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="59">
   <si>
     <t>Beschreibung</t>
   </si>
@@ -198,6 +205,12 @@
   </si>
   <si>
     <t>Servo Posiu Rechts</t>
+  </si>
+  <si>
+    <t>Data Bytes - Dec</t>
+  </si>
+  <si>
+    <t>Servo Posi Rechts</t>
   </si>
 </sst>
 </file>
@@ -1916,7 +1929,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:Z8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1932,7 +1945,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B1" s="31" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
@@ -2691,7 +2704,7 @@
     </row>
     <row r="11" spans="1:27" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B11" s="9">
         <v>1</v>
@@ -2807,271 +2820,275 @@
       <c r="Z12" s="20"/>
     </row>
     <row r="13" spans="1:27" s="25" customFormat="1" ht="102" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" s="24" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="O13" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="P13" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="S13" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="T13" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="U13" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="V13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="W13" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="X13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z13" s="24" t="s">
+      <c r="N13"/>
+      <c r="O13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:27" s="25" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="26">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="9">
         <v>4</v>
       </c>
-      <c r="C14" s="27">
-        <v>0</v>
-      </c>
-      <c r="D14" s="27">
-        <v>0</v>
-      </c>
-      <c r="E14" s="27">
-        <v>80</v>
-      </c>
-      <c r="F14" s="27">
-        <v>100</v>
-      </c>
-      <c r="G14" s="27">
-        <v>128</v>
-      </c>
-      <c r="H14" s="27">
-        <v>128</v>
-      </c>
-      <c r="I14" s="27">
-        <v>100</v>
-      </c>
-      <c r="J14" s="27">
-        <v>80</v>
-      </c>
-      <c r="K14" s="27">
-        <v>0</v>
-      </c>
-      <c r="L14" s="27">
-        <v>0</v>
-      </c>
-      <c r="M14" s="28">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="12">
         <f>_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(C14,D14),E14),F14),G14),H14),I14),J14),K14),L14)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="26" t="str">
+      <c r="N14" s="1"/>
+      <c r="O14" s="9" t="str">
         <f>DEC2HEX(B14,2)</f>
         <v>04</v>
       </c>
-      <c r="P14" s="27" t="str">
+      <c r="P14" s="7" t="str">
         <f>DEC2HEX(C14,2)</f>
         <v>00</v>
       </c>
-      <c r="Q14" s="27" t="str">
+      <c r="Q14" s="7" t="str">
         <f t="shared" ref="Q14:Y14" si="17">DEC2HEX(D14,2)</f>
         <v>00</v>
       </c>
-      <c r="R14" s="27" t="str">
+      <c r="R14" s="7" t="str">
         <f t="shared" si="17"/>
-        <v>50</v>
-      </c>
-      <c r="S14" s="27" t="str">
+        <v>00</v>
+      </c>
+      <c r="S14" s="7" t="str">
         <f t="shared" si="17"/>
-        <v>64</v>
-      </c>
-      <c r="T14" s="27" t="str">
+        <v>00</v>
+      </c>
+      <c r="T14" s="7" t="str">
         <f t="shared" si="17"/>
+        <v>00</v>
+      </c>
+      <c r="U14" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>00</v>
+      </c>
+      <c r="V14" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>00</v>
+      </c>
+      <c r="W14" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>00</v>
+      </c>
+      <c r="X14" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>00</v>
+      </c>
+      <c r="Y14" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>00</v>
+      </c>
+      <c r="Z14" s="12" t="str">
+        <f>DEC2HEX(M14,2)</f>
+        <v>00</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="102" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="25"/>
+      <c r="O15" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="S15" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="V15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="W15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="X15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y15" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z15" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="1" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="26">
+        <v>5</v>
+      </c>
+      <c r="C16" s="27">
+        <v>0</v>
+      </c>
+      <c r="D16" s="27">
+        <v>0</v>
+      </c>
+      <c r="E16" s="27">
         <v>80</v>
       </c>
-      <c r="U14" s="27" t="str">
-        <f t="shared" si="17"/>
+      <c r="F16" s="27">
+        <v>100</v>
+      </c>
+      <c r="G16" s="27">
+        <v>128</v>
+      </c>
+      <c r="H16" s="27">
+        <v>128</v>
+      </c>
+      <c r="I16" s="27">
+        <v>100</v>
+      </c>
+      <c r="J16" s="27">
         <v>80</v>
       </c>
-      <c r="V14" s="27" t="str">
-        <f t="shared" si="17"/>
-        <v>64</v>
-      </c>
-      <c r="W14" s="27" t="str">
-        <f t="shared" si="17"/>
-        <v>50</v>
-      </c>
-      <c r="X14" s="27" t="str">
-        <f t="shared" si="17"/>
-        <v>00</v>
-      </c>
-      <c r="Y14" s="27" t="str">
-        <f t="shared" si="17"/>
-        <v>00</v>
-      </c>
-      <c r="Z14" s="28" t="str">
-        <f>DEC2HEX(M14,2)</f>
-        <v>00</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="102" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="5"/>
-      <c r="W15" s="5"/>
-      <c r="X15" s="5"/>
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="9">
-        <v>5</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="12">
+      <c r="K16" s="27">
+        <v>0</v>
+      </c>
+      <c r="L16" s="27">
+        <v>0</v>
+      </c>
+      <c r="M16" s="28">
         <f>_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(_xlfn.BITXOR(C16,D16),E16),F16),G16),H16),I16),J16),K16),L16)</f>
         <v>0</v>
       </c>
-      <c r="O16" s="9" t="str">
+      <c r="N16" s="25"/>
+      <c r="O16" s="26" t="str">
         <f>DEC2HEX(B16,2)</f>
         <v>05</v>
       </c>
-      <c r="P16" s="7" t="str">
+      <c r="P16" s="27" t="str">
         <f>DEC2HEX(C16,2)</f>
         <v>00</v>
       </c>
-      <c r="Q16" s="7" t="str">
+      <c r="Q16" s="27" t="str">
         <f t="shared" ref="Q16:Y16" si="18">DEC2HEX(D16,2)</f>
         <v>00</v>
       </c>
-      <c r="R16" s="7" t="str">
+      <c r="R16" s="27" t="str">
         <f t="shared" si="18"/>
-        <v>00</v>
-      </c>
-      <c r="S16" s="7" t="str">
+        <v>50</v>
+      </c>
+      <c r="S16" s="27" t="str">
         <f t="shared" si="18"/>
-        <v>00</v>
-      </c>
-      <c r="T16" s="7" t="str">
+        <v>64</v>
+      </c>
+      <c r="T16" s="27" t="str">
         <f t="shared" si="18"/>
-        <v>00</v>
-      </c>
-      <c r="U16" s="7" t="str">
+        <v>80</v>
+      </c>
+      <c r="U16" s="27" t="str">
         <f t="shared" si="18"/>
-        <v>00</v>
-      </c>
-      <c r="V16" s="7" t="str">
+        <v>80</v>
+      </c>
+      <c r="V16" s="27" t="str">
         <f t="shared" si="18"/>
-        <v>00</v>
-      </c>
-      <c r="W16" s="7" t="str">
+        <v>64</v>
+      </c>
+      <c r="W16" s="27" t="str">
         <f t="shared" si="18"/>
-        <v>00</v>
-      </c>
-      <c r="X16" s="7" t="str">
+        <v>50</v>
+      </c>
+      <c r="X16" s="27" t="str">
         <f t="shared" si="18"/>
         <v>00</v>
       </c>
-      <c r="Y16" s="7" t="str">
+      <c r="Y16" s="27" t="str">
         <f t="shared" si="18"/>
         <v>00</v>
       </c>
-      <c r="Z16" s="12" t="str">
+      <c r="Z16" s="28" t="str">
         <f>DEC2HEX(M16,2)</f>
         <v>00</v>
       </c>

</xml_diff>